<commit_message>
Mail doku fertig Karic
</commit_message>
<xml_diff>
--- a/Protokolle/Arbeitsaufteilung.xlsx
+++ b/Protokolle/Arbeitsaufteilung.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\LDAP\Protokolle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adin Karic\Desktop\pp\LDAP\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16242" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16245" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -147,6 +147,33 @@
   </si>
   <si>
     <t>120min</t>
+  </si>
+  <si>
+    <t>benötigt iRedMail Pro</t>
+  </si>
+  <si>
+    <t>360min</t>
+  </si>
+  <si>
+    <t>teilweise schon integriert</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Mailserver verbinden mit LDAP Server</t>
+  </si>
+  <si>
+    <t>Tutorial gefunden aber nicht möglich</t>
+  </si>
+  <si>
+    <t>14.03.2015 ff.</t>
+  </si>
+  <si>
+    <t>200 min</t>
+  </si>
+  <si>
+    <t>15 min</t>
   </si>
 </sst>
 </file>
@@ -228,17 +255,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -254,8 +281,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B3:F32" totalsRowShown="0">
-  <autoFilter ref="B3:F32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B3:F33" totalsRowShown="0">
+  <autoFilter ref="B3:F33"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Aufgaben"/>
     <tableColumn id="2" name="Wer(Adler, Karic, Kopec)"/>
@@ -589,19 +616,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F32"/>
+  <dimension ref="B3:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="103.6484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6484375" customWidth="1"/>
-    <col min="4" max="4" width="11.34765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.84765625" customWidth="1"/>
-    <col min="6" max="6" width="21.84765625" customWidth="1"/>
+    <col min="2" max="2" width="103.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
@@ -633,79 +660,109 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="2">
-        <v>42059</v>
+        <v>42073</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>42084</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="1" t="s">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2">
+        <v>42080</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2">
-        <v>42072</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" t="s">
-        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
+      <c r="D10" s="2">
+        <v>42072</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="2:6">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>42087</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2">
-        <v>42072</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
       </c>
       <c r="F14" t="s">
         <v>33</v>
@@ -713,135 +770,152 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42072</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
-        <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="2">
-        <v>42059</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2">
+        <v>42059</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2">
-        <v>42060</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2">
+        <v>42060</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="2:6">
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D26" s="2">
         <v>42072</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>32</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="2:6">
+      <c r="B28" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="2">
-        <v>42073</v>
-      </c>
-      <c r="E29" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="2">
+        <v>42073</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="2">
         <v>42069</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>31</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="5" t="s">
+    <row r="33" spans="2:6">
+      <c r="B33" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D33" s="4">
         <v>42080</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>